<commit_message>
BACKEND-2 test carga masiva tfgs hechos y esqueleto doc de código
</commit_message>
<xml_diff>
--- a/apps/controller/ws/tests/test_upload_file_tfgs/ListaTFGs.xlsx
+++ b/apps/controller/ws/tests/test_upload_file_tfgs/ListaTFGs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="938">
   <si>
     <r>
       <t xml:space="preserve">Nota</t>
@@ -139,9 +139,6 @@
     <t>miguelgarcia@ugr.es</t>
   </si>
   <si>
-    <t>Programación de un robot usando python y pyro</t>
-  </si>
-  <si>
     <t>El objetivo es el desarrollo de una aplicación usando python que permite realizar algunas tareas básicas con un robot Peoplebot. Para ello se utilizara como método inicial de trabajo el simulador proporcionado por pyro y a continuación se probará su funcionamiento sobre el robot real.</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>Miguel García Silvente</t>
+  </si>
+  <si>
+    <t>Programación de un robot usando python y pyro</t>
   </si>
   <si>
     <t>Francisco Herrera Triguero</t>
@@ -3732,7 +3732,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -4816,6 +4816,99 @@
       <c r="I5" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
+      <c r="BR5" s="0"/>
+      <c r="BS5" s="0"/>
+      <c r="BT5" s="0"/>
+      <c r="BU5" s="0"/>
+      <c r="BV5" s="0"/>
+      <c r="BW5" s="0"/>
+      <c r="BX5" s="0"/>
+      <c r="BY5" s="0"/>
+      <c r="BZ5" s="0"/>
+      <c r="CA5" s="0"/>
+      <c r="CB5" s="0"/>
+      <c r="CC5" s="0"/>
+      <c r="CD5" s="0"/>
+      <c r="CE5" s="0"/>
+      <c r="CF5" s="0"/>
+      <c r="CG5" s="0"/>
+      <c r="CH5" s="0"/>
+      <c r="CI5" s="0"/>
+      <c r="CJ5" s="0"/>
+      <c r="CK5" s="0"/>
+      <c r="CL5" s="0"/>
+      <c r="CM5" s="0"/>
+      <c r="CN5" s="0"/>
+      <c r="CO5" s="0"/>
+      <c r="CP5" s="0"/>
+      <c r="CQ5" s="0"/>
+      <c r="CR5" s="0"/>
+      <c r="CS5" s="0"/>
+      <c r="CT5" s="0"/>
+      <c r="CU5" s="0"/>
+      <c r="CV5" s="0"/>
+      <c r="CW5" s="0"/>
+      <c r="CX5" s="0"/>
       <c r="CY5" s="0"/>
       <c r="CZ5" s="0"/>
       <c r="DA5" s="0"/>
@@ -4973,9 +5066,7 @@
         <f aca="false">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
         <v>11</v>
@@ -4995,6 +5086,99 @@
       <c r="I6" s="17" t="s">
         <v>14</v>
       </c>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
+      <c r="AF6" s="0"/>
+      <c r="AG6" s="0"/>
+      <c r="AH6" s="0"/>
+      <c r="AI6" s="0"/>
+      <c r="AJ6" s="0"/>
+      <c r="AK6" s="0"/>
+      <c r="AL6" s="0"/>
+      <c r="AM6" s="0"/>
+      <c r="AN6" s="0"/>
+      <c r="AO6" s="0"/>
+      <c r="AP6" s="0"/>
+      <c r="AQ6" s="0"/>
+      <c r="AR6" s="0"/>
+      <c r="AS6" s="0"/>
+      <c r="AT6" s="0"/>
+      <c r="AU6" s="0"/>
+      <c r="AV6" s="0"/>
+      <c r="AW6" s="0"/>
+      <c r="AX6" s="0"/>
+      <c r="AY6" s="0"/>
+      <c r="AZ6" s="0"/>
+      <c r="BA6" s="0"/>
+      <c r="BB6" s="0"/>
+      <c r="BC6" s="0"/>
+      <c r="BD6" s="0"/>
+      <c r="BE6" s="0"/>
+      <c r="BF6" s="0"/>
+      <c r="BG6" s="0"/>
+      <c r="BH6" s="0"/>
+      <c r="BI6" s="0"/>
+      <c r="BJ6" s="0"/>
+      <c r="BK6" s="0"/>
+      <c r="BL6" s="0"/>
+      <c r="BM6" s="0"/>
+      <c r="BN6" s="0"/>
+      <c r="BO6" s="0"/>
+      <c r="BP6" s="0"/>
+      <c r="BQ6" s="0"/>
+      <c r="BR6" s="0"/>
+      <c r="BS6" s="0"/>
+      <c r="BT6" s="0"/>
+      <c r="BU6" s="0"/>
+      <c r="BV6" s="0"/>
+      <c r="BW6" s="0"/>
+      <c r="BX6" s="0"/>
+      <c r="BY6" s="0"/>
+      <c r="BZ6" s="0"/>
+      <c r="CA6" s="0"/>
+      <c r="CB6" s="0"/>
+      <c r="CC6" s="0"/>
+      <c r="CD6" s="0"/>
+      <c r="CE6" s="0"/>
+      <c r="CF6" s="0"/>
+      <c r="CG6" s="0"/>
+      <c r="CH6" s="0"/>
+      <c r="CI6" s="0"/>
+      <c r="CJ6" s="0"/>
+      <c r="CK6" s="0"/>
+      <c r="CL6" s="0"/>
+      <c r="CM6" s="0"/>
+      <c r="CN6" s="0"/>
+      <c r="CO6" s="0"/>
+      <c r="CP6" s="0"/>
+      <c r="CQ6" s="0"/>
+      <c r="CR6" s="0"/>
+      <c r="CS6" s="0"/>
+      <c r="CT6" s="0"/>
+      <c r="CU6" s="0"/>
+      <c r="CV6" s="0"/>
+      <c r="CW6" s="0"/>
+      <c r="CX6" s="0"/>
       <c r="CY6" s="0"/>
       <c r="CZ6" s="0"/>
       <c r="DA6" s="0"/>
@@ -5147,7 +5331,7 @@
       <c r="IR6" s="0"/>
       <c r="IS6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="n">
         <f aca="false">A6+1</f>
         <v>3</v>
@@ -5172,6 +5356,99 @@
       <c r="I7" s="23" t="s">
         <v>20</v>
       </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="0"/>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
+      <c r="AO7" s="0"/>
+      <c r="AP7" s="0"/>
+      <c r="AQ7" s="0"/>
+      <c r="AR7" s="0"/>
+      <c r="AS7" s="0"/>
+      <c r="AT7" s="0"/>
+      <c r="AU7" s="0"/>
+      <c r="AV7" s="0"/>
+      <c r="AW7" s="0"/>
+      <c r="AX7" s="0"/>
+      <c r="AY7" s="0"/>
+      <c r="AZ7" s="0"/>
+      <c r="BA7" s="0"/>
+      <c r="BB7" s="0"/>
+      <c r="BC7" s="0"/>
+      <c r="BD7" s="0"/>
+      <c r="BE7" s="0"/>
+      <c r="BF7" s="0"/>
+      <c r="BG7" s="0"/>
+      <c r="BH7" s="0"/>
+      <c r="BI7" s="0"/>
+      <c r="BJ7" s="0"/>
+      <c r="BK7" s="0"/>
+      <c r="BL7" s="0"/>
+      <c r="BM7" s="0"/>
+      <c r="BN7" s="0"/>
+      <c r="BO7" s="0"/>
+      <c r="BP7" s="0"/>
+      <c r="BQ7" s="0"/>
+      <c r="BR7" s="0"/>
+      <c r="BS7" s="0"/>
+      <c r="BT7" s="0"/>
+      <c r="BU7" s="0"/>
+      <c r="BV7" s="0"/>
+      <c r="BW7" s="0"/>
+      <c r="BX7" s="0"/>
+      <c r="BY7" s="0"/>
+      <c r="BZ7" s="0"/>
+      <c r="CA7" s="0"/>
+      <c r="CB7" s="0"/>
+      <c r="CC7" s="0"/>
+      <c r="CD7" s="0"/>
+      <c r="CE7" s="0"/>
+      <c r="CF7" s="0"/>
+      <c r="CG7" s="0"/>
+      <c r="CH7" s="0"/>
+      <c r="CI7" s="0"/>
+      <c r="CJ7" s="0"/>
+      <c r="CK7" s="0"/>
+      <c r="CL7" s="0"/>
+      <c r="CM7" s="0"/>
+      <c r="CN7" s="0"/>
+      <c r="CO7" s="0"/>
+      <c r="CP7" s="0"/>
+      <c r="CQ7" s="0"/>
+      <c r="CR7" s="0"/>
+      <c r="CS7" s="0"/>
+      <c r="CT7" s="0"/>
+      <c r="CU7" s="0"/>
+      <c r="CV7" s="0"/>
+      <c r="CW7" s="0"/>
+      <c r="CX7" s="0"/>
       <c r="CY7" s="0"/>
       <c r="CZ7" s="0"/>
       <c r="DA7" s="0"/>
@@ -5324,7 +5601,7 @@
       <c r="IR7" s="0"/>
       <c r="IS7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="n">
         <f aca="false">A7+1</f>
         <v>4</v>
@@ -5338,19 +5615,110 @@
       <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="E8" s="14"/>
       <c r="F8" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
+      <c r="AG8" s="0"/>
+      <c r="AH8" s="0"/>
+      <c r="AI8" s="0"/>
+      <c r="AJ8" s="0"/>
+      <c r="AK8" s="0"/>
+      <c r="AL8" s="0"/>
+      <c r="AM8" s="0"/>
+      <c r="AN8" s="0"/>
+      <c r="AO8" s="0"/>
+      <c r="AP8" s="0"/>
+      <c r="AQ8" s="0"/>
+      <c r="AR8" s="0"/>
+      <c r="AS8" s="0"/>
+      <c r="AT8" s="0"/>
+      <c r="AU8" s="0"/>
+      <c r="AV8" s="0"/>
+      <c r="AW8" s="0"/>
+      <c r="AX8" s="0"/>
+      <c r="AY8" s="0"/>
+      <c r="AZ8" s="0"/>
+      <c r="BA8" s="0"/>
+      <c r="BB8" s="0"/>
+      <c r="BC8" s="0"/>
+      <c r="BD8" s="0"/>
+      <c r="BE8" s="0"/>
+      <c r="BF8" s="0"/>
+      <c r="BG8" s="0"/>
+      <c r="BH8" s="0"/>
+      <c r="BI8" s="0"/>
+      <c r="BJ8" s="0"/>
+      <c r="BK8" s="0"/>
+      <c r="BL8" s="0"/>
+      <c r="BM8" s="0"/>
+      <c r="BN8" s="0"/>
+      <c r="BO8" s="0"/>
+      <c r="BP8" s="0"/>
+      <c r="BQ8" s="0"/>
+      <c r="BR8" s="0"/>
+      <c r="BS8" s="0"/>
+      <c r="BT8" s="0"/>
+      <c r="BU8" s="0"/>
+      <c r="BV8" s="0"/>
+      <c r="BW8" s="0"/>
+      <c r="BX8" s="0"/>
+      <c r="BY8" s="0"/>
+      <c r="BZ8" s="0"/>
+      <c r="CA8" s="0"/>
+      <c r="CB8" s="0"/>
+      <c r="CC8" s="0"/>
+      <c r="CD8" s="0"/>
+      <c r="CE8" s="0"/>
+      <c r="CF8" s="0"/>
+      <c r="CG8" s="0"/>
+      <c r="CH8" s="0"/>
+      <c r="CI8" s="0"/>
+      <c r="CJ8" s="0"/>
+      <c r="CK8" s="0"/>
+      <c r="CL8" s="0"/>
+      <c r="CM8" s="0"/>
+      <c r="CN8" s="0"/>
+      <c r="CO8" s="0"/>
+      <c r="CP8" s="0"/>
+      <c r="CQ8" s="0"/>
+      <c r="CR8" s="0"/>
+      <c r="CS8" s="0"/>
+      <c r="CT8" s="0"/>
+      <c r="CU8" s="0"/>
+      <c r="CV8" s="0"/>
+      <c r="CW8" s="0"/>
+      <c r="CX8" s="0"/>
       <c r="CY8" s="0"/>
       <c r="CZ8" s="0"/>
       <c r="DA8" s="0"/>
@@ -5503,31 +5871,31 @@
       <c r="IR8" s="0"/>
       <c r="IS8" s="0"/>
     </row>
-    <row r="9" s="24" customFormat="true" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="24" customFormat="true" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="n">
         <f aca="false">A8+1</f>
         <v>5</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="21" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="23"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -6021,16 +6389,18 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="jorgecasillas@ugr.es"/>
-    <hyperlink ref="B6" r:id="rId2" display="jorgecasillas@ugr.es"/>
-    <hyperlink ref="B7" r:id="rId3" display="juanmanuelfernandez@ugr.es"/>
-    <hyperlink ref="B8" r:id="rId4" display="eugenioaguirre@ugr.es"/>
-    <hyperlink ref="C8" r:id="rId5" display="miguelgarcia@ugr.es"/>
-    <hyperlink ref="B9" r:id="rId6" display="franciscoherrera@ugr.es"/>
+    <hyperlink ref="B7" r:id="rId2" display="juanmanuelfernandez@ugr.es"/>
+    <hyperlink ref="B8" r:id="rId3" display="eugenioaguirre@ugr.es"/>
+    <hyperlink ref="C8" r:id="rId4" display="miguelgarcia@ugr.es"/>
+    <hyperlink ref="B9" r:id="rId5" display="franciscoherrera@ugr.es"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.0784722222222222" right="0.0784722222222222" top="0.493055555555556" bottom="0.493055555555556" header="0.354166666666667" footer="0.354166666666667"/>
@@ -6075,7 +6445,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="293.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="26" t="s">
@@ -6085,7 +6455,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="27" t="n">
         <v>1</v>
@@ -6350,7 +6720,7 @@
     </row>
     <row r="2" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="26" t="s">
@@ -6360,7 +6730,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="27" t="n">
         <v>1</v>
@@ -6625,10 +6995,10 @@
     </row>
     <row r="3" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>33</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>11</v>
@@ -6637,7 +7007,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="27" t="n">
         <v>1</v>
@@ -6900,19 +7270,19 @@
     </row>
     <row r="4" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>35</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="27" t="n">
         <v>1</v>
@@ -6922,10 +7292,10 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="25" t="s">
         <v>24</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>25</v>
       </c>
       <c r="M4" s="25"/>
       <c r="N4" s="0"/>
@@ -7185,7 +7555,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="30" t="n">
         <v>1</v>
@@ -7195,10 +7565,10 @@
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
       <c r="K5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="28" t="s">
         <v>28</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>29</v>
       </c>
       <c r="M5" s="28"/>
     </row>
@@ -7216,7 +7586,7 @@
         <v>40</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="27" t="n">
         <v>1</v>
@@ -7493,7 +7863,7 @@
         <v>44</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="27" t="n">
         <v>1</v>
@@ -7766,7 +8136,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="27" t="n">
         <v>1</v>
@@ -8037,7 +8407,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="27" t="n">
         <v>1</v>
@@ -8308,7 +8678,7 @@
         <v>52</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="27" t="n">
         <v>1</v>
@@ -8335,7 +8705,7 @@
         <v>55</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="27" t="n">
         <v>2</v>
@@ -8610,7 +8980,7 @@
         <v>59</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="27" t="n">
         <v>1</v>
@@ -8885,7 +9255,7 @@
         <v>65</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="27" t="n">
         <v>1</v>
@@ -9162,7 +9532,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="27" t="n">
         <v>1</v>
@@ -9437,7 +9807,7 @@
         <v>74</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="27" t="n">
         <v>1</v>
@@ -9710,7 +10080,7 @@
         <v>77</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="27" t="n">
         <v>1</v>
@@ -9983,7 +10353,7 @@
         <v>81</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="27" t="n">
         <v>1</v>
@@ -11079,7 +11449,7 @@
     </row>
     <row r="21" customFormat="false" ht="216.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>36</v>
@@ -11914,10 +12284,10 @@
     </row>
     <row r="24" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>34</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>35</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>11</v>
@@ -12195,7 +12565,7 @@
     </row>
     <row r="25" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>125</v>
@@ -12476,7 +12846,7 @@
     </row>
     <row r="26" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26" t="s">
@@ -12755,7 +13125,7 @@
     </row>
     <row r="27" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="26" t="s">
@@ -13034,7 +13404,7 @@
     </row>
     <row r="28" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="26" t="s">
@@ -13348,7 +13718,7 @@
     </row>
     <row r="30" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>155</v>
@@ -13629,7 +13999,7 @@
     </row>
     <row r="31" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="26"/>
@@ -20163,7 +20533,7 @@
         <v>440</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F89" s="25" t="n">
         <v>1</v>
@@ -20192,7 +20562,7 @@
         <v>444</v>
       </c>
       <c r="E90" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F90" s="25" t="n">
         <v>1</v>
@@ -20221,7 +20591,7 @@
         <v>448</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F91" s="25" t="n">
         <v>1</v>
@@ -20250,7 +20620,7 @@
         <v>452</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F92" s="25" t="n">
         <v>1</v>
@@ -20279,7 +20649,7 @@
         <v>455</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F93" s="25" t="n">
         <v>1</v>
@@ -20308,7 +20678,7 @@
         <v>457</v>
       </c>
       <c r="E94" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F94" s="25" t="n">
         <v>1</v>
@@ -20783,7 +21153,7 @@
         <v>520</v>
       </c>
       <c r="E109" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F109" s="28" t="n">
         <v>1</v>
@@ -23357,6 +23727,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -23609,6 +23982,9 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -32249,6 +32625,15 @@
       <c r="J38" s="80" t="s">
         <v>632</v>
       </c>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
+      <c r="N38" s="0"/>
+      <c r="O38" s="0"/>
+      <c r="P38" s="0"/>
+      <c r="Q38" s="0"/>
+      <c r="R38" s="0"/>
+      <c r="S38" s="0"/>
       <c r="T38" s="0"/>
       <c r="U38" s="0"/>
       <c r="V38" s="0"/>
@@ -32513,6 +32898,15 @@
       <c r="J39" s="84" t="s">
         <v>639</v>
       </c>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="N39" s="0"/>
+      <c r="O39" s="0"/>
+      <c r="P39" s="0"/>
+      <c r="Q39" s="0"/>
+      <c r="R39" s="0"/>
+      <c r="S39" s="0"/>
       <c r="T39" s="0"/>
       <c r="U39" s="0"/>
       <c r="V39" s="0"/>
@@ -32777,6 +33171,15 @@
       <c r="J40" s="80" t="s">
         <v>652</v>
       </c>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
+      <c r="N40" s="0"/>
+      <c r="O40" s="0"/>
+      <c r="P40" s="0"/>
+      <c r="Q40" s="0"/>
+      <c r="R40" s="0"/>
+      <c r="S40" s="0"/>
       <c r="T40" s="0"/>
       <c r="U40" s="0"/>
       <c r="V40" s="0"/>
@@ -33631,6 +34034,18 @@
       <c r="J44" s="80" t="s">
         <v>680</v>
       </c>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
+      <c r="N44" s="0"/>
+      <c r="O44" s="0"/>
+      <c r="P44" s="0"/>
+      <c r="Q44" s="0"/>
+      <c r="R44" s="0"/>
+      <c r="S44" s="0"/>
+      <c r="T44" s="0"/>
+      <c r="U44" s="0"/>
+      <c r="V44" s="0"/>
       <c r="W44" s="0"/>
       <c r="X44" s="0"/>
       <c r="Y44" s="0"/>
@@ -33894,6 +34309,18 @@
       <c r="J45" s="84" t="s">
         <v>689</v>
       </c>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="O45" s="0"/>
+      <c r="P45" s="0"/>
+      <c r="Q45" s="0"/>
+      <c r="R45" s="0"/>
+      <c r="S45" s="0"/>
+      <c r="T45" s="0"/>
+      <c r="U45" s="0"/>
+      <c r="V45" s="0"/>
       <c r="W45" s="0"/>
       <c r="X45" s="0"/>
       <c r="Y45" s="0"/>
@@ -34155,6 +34582,10 @@
       <c r="J46" s="80" t="s">
         <v>694</v>
       </c>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="N46" s="0"/>
       <c r="O46" s="0"/>
       <c r="P46" s="0"/>
       <c r="Q46" s="0"/>
@@ -35822,6 +36253,10 @@
         <v>738</v>
       </c>
       <c r="J53" s="84"/>
+      <c r="K53" s="0"/>
+      <c r="L53" s="0"/>
+      <c r="M53" s="0"/>
+      <c r="N53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="191.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="77" t="n">
@@ -35851,6 +36286,10 @@
       <c r="J54" s="80" t="s">
         <v>744</v>
       </c>
+      <c r="K54" s="0"/>
+      <c r="L54" s="0"/>
+      <c r="M54" s="0"/>
+      <c r="N54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="81" t="n">
@@ -35880,6 +36319,10 @@
       <c r="J55" s="84" t="s">
         <v>734</v>
       </c>
+      <c r="K55" s="0"/>
+      <c r="L55" s="0"/>
+      <c r="M55" s="0"/>
+      <c r="N55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="270" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="77" t="n">
@@ -35909,6 +36352,10 @@
       <c r="J56" s="80" t="s">
         <v>756</v>
       </c>
+      <c r="K56" s="0"/>
+      <c r="L56" s="0"/>
+      <c r="M56" s="0"/>
+      <c r="N56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="81" t="n">
@@ -35938,6 +36385,10 @@
       <c r="J57" s="84" t="s">
         <v>763</v>
       </c>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="N57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="77" t="n">
@@ -35967,6 +36418,10 @@
       <c r="J58" s="80" t="s">
         <v>768</v>
       </c>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+      <c r="M58" s="0"/>
+      <c r="N58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="303.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="81" t="n">
@@ -36075,7 +36530,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>36</v>
@@ -36172,10 +36627,10 @@
         <v>61</v>
       </c>
       <c r="B65" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="C65" s="19" t="s">
-        <v>35</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>11</v>
@@ -36207,7 +36662,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>125</v>
@@ -36242,7 +36697,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19" t="s">
@@ -36275,7 +36730,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13" t="s">
@@ -36308,7 +36763,7 @@
         <v>65</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="19" t="s">
@@ -36341,7 +36796,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>155</v>
@@ -36376,7 +36831,7 @@
         <v>67</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -37154,6 +37609,7 @@
       <c r="J95" s="84" t="s">
         <v>58</v>
       </c>
+      <c r="K95" s="0"/>
       <c r="L95" s="0"/>
       <c r="M95" s="0"/>
       <c r="N95" s="0"/>
@@ -37717,7 +38173,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>1</v>
@@ -37730,26 +38186,28 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="13"/>
-      <c r="D2" s="0" t="e">
+      <c r="D2" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C2,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">VLOOKUP(C3,A:B,2,0)</f>
@@ -37758,13 +38216,13 @@
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">VLOOKUP(C4,A:B,2,0)</f>
@@ -37773,15 +38231,17 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="0" t="e">
+      <c r="D5" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C5,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37822,9 +38282,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="0" t="e">
+      <c r="D8" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C8,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37835,9 +38297,11 @@
         <v>9</v>
       </c>
       <c r="C9" s="19"/>
-      <c r="D9" s="0" t="e">
+      <c r="D9" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C9,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37848,9 +38312,11 @@
         <v>10</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="0" t="e">
+      <c r="D10" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C10,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37861,9 +38327,11 @@
         <v>11</v>
       </c>
       <c r="C11" s="19"/>
-      <c r="D11" s="0" t="e">
+      <c r="D11" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C11,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37874,9 +38342,11 @@
         <v>12</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="0" t="e">
+      <c r="D12" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C12,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37887,9 +38357,11 @@
         <v>13</v>
       </c>
       <c r="C13" s="19"/>
-      <c r="D13" s="0" t="e">
+      <c r="D13" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C13,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37915,9 +38387,11 @@
         <v>15</v>
       </c>
       <c r="C15" s="19"/>
-      <c r="D15" s="0" t="e">
+      <c r="D15" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C15,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37928,9 +38402,11 @@
         <v>16</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="0" t="e">
+      <c r="D16" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C16,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37941,9 +38417,11 @@
         <v>17</v>
       </c>
       <c r="C17" s="19"/>
-      <c r="D17" s="0" t="e">
+      <c r="D17" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C17,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37956,9 +38434,11 @@
       <c r="C18" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D18" s="0" t="e">
+      <c r="D18" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C18,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="19" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37999,9 +38479,11 @@
         <v>21</v>
       </c>
       <c r="C21" s="19"/>
-      <c r="D21" s="0" t="e">
+      <c r="D21" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C21,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38012,9 +38494,11 @@
         <v>22</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="0" t="e">
+      <c r="D22" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C22,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38025,9 +38509,11 @@
         <v>23</v>
       </c>
       <c r="C23" s="19"/>
-      <c r="D23" s="0" t="e">
+      <c r="D23" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C23,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38038,9 +38524,11 @@
         <v>24</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="0" t="e">
+      <c r="D24" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C24,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38051,9 +38539,11 @@
         <v>25</v>
       </c>
       <c r="C25" s="19"/>
-      <c r="D25" s="0" t="e">
+      <c r="D25" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C25,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38064,9 +38554,11 @@
         <v>26</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="0" t="e">
+      <c r="D26" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C26,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38077,9 +38569,11 @@
         <v>27</v>
       </c>
       <c r="C27" s="19"/>
-      <c r="D27" s="0" t="e">
+      <c r="D27" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C27,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38090,9 +38584,11 @@
         <v>28</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="0" t="e">
+      <c r="D28" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C28,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38103,9 +38599,11 @@
         <v>29</v>
       </c>
       <c r="C29" s="19"/>
-      <c r="D29" s="0" t="e">
+      <c r="D29" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C29,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38116,9 +38614,11 @@
         <v>30</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="0" t="e">
+      <c r="D30" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C30,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38129,9 +38629,11 @@
         <v>31</v>
       </c>
       <c r="C31" s="19"/>
-      <c r="D31" s="0" t="e">
+      <c r="D31" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C31,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38157,9 +38659,11 @@
         <v>33</v>
       </c>
       <c r="C33" s="19"/>
-      <c r="D33" s="0" t="e">
+      <c r="D33" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C33,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38172,9 +38676,11 @@
       <c r="C34" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="D34" s="0" t="e">
+      <c r="D34" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C34,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38185,9 +38691,11 @@
         <v>35</v>
       </c>
       <c r="C35" s="19"/>
-      <c r="D35" s="0" t="e">
+      <c r="D35" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C35,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38198,9 +38706,11 @@
         <v>36</v>
       </c>
       <c r="C36" s="13"/>
-      <c r="D36" s="0" t="e">
+      <c r="D36" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C36,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38211,9 +38721,11 @@
         <v>37</v>
       </c>
       <c r="C37" s="19"/>
-      <c r="D37" s="0" t="e">
+      <c r="D37" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C37,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38224,9 +38736,11 @@
         <v>38</v>
       </c>
       <c r="C38" s="13"/>
-      <c r="D38" s="0" t="e">
+      <c r="D38" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C38,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38237,9 +38751,11 @@
         <v>39</v>
       </c>
       <c r="C39" s="19"/>
-      <c r="D39" s="0" t="e">
+      <c r="D39" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C39,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38250,9 +38766,11 @@
         <v>40</v>
       </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="0" t="e">
+      <c r="D40" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C40,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38263,9 +38781,11 @@
         <v>41</v>
       </c>
       <c r="C41" s="19"/>
-      <c r="D41" s="0" t="e">
+      <c r="D41" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C41,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38276,9 +38796,11 @@
         <v>42</v>
       </c>
       <c r="C42" s="13"/>
-      <c r="D42" s="0" t="e">
+      <c r="D42" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C42,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38289,9 +38811,11 @@
         <v>43</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="0" t="e">
+      <c r="D43" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C43,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38347,9 +38871,11 @@
         <v>47</v>
       </c>
       <c r="C47" s="19"/>
-      <c r="D47" s="0" t="e">
+      <c r="D47" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C47,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38360,9 +38886,11 @@
         <v>48</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="0" t="e">
+      <c r="D48" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C48,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38373,9 +38901,11 @@
         <v>49</v>
       </c>
       <c r="C49" s="19"/>
-      <c r="D49" s="0" t="e">
+      <c r="D49" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C49,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="50" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38416,9 +38946,11 @@
         <v>52</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="0" t="e">
+      <c r="D52" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C52,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38429,9 +38961,11 @@
         <v>53</v>
       </c>
       <c r="C53" s="19"/>
-      <c r="D53" s="0" t="e">
+      <c r="D53" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C53,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38442,9 +38976,11 @@
         <v>54</v>
       </c>
       <c r="C54" s="13"/>
-      <c r="D54" s="0" t="e">
+      <c r="D54" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C54,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38455,9 +38991,11 @@
         <v>55</v>
       </c>
       <c r="C55" s="19"/>
-      <c r="D55" s="0" t="e">
+      <c r="D55" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C55,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38468,9 +39006,11 @@
         <v>56</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="0" t="e">
+      <c r="D56" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C56,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38481,9 +39021,11 @@
         <v>57</v>
       </c>
       <c r="C57" s="19"/>
-      <c r="D57" s="0" t="e">
+      <c r="D57" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C57,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38494,9 +39036,11 @@
         <v>58</v>
       </c>
       <c r="C58" s="13"/>
-      <c r="D58" s="0" t="e">
+      <c r="D58" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C58,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38507,9 +39051,11 @@
         <v>59</v>
       </c>
       <c r="C59" s="19"/>
-      <c r="D59" s="0" t="e">
+      <c r="D59" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C59,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38520,9 +39066,11 @@
         <v>60</v>
       </c>
       <c r="C60" s="13"/>
-      <c r="D60" s="0" t="e">
+      <c r="D60" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C60,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38533,9 +39081,11 @@
         <v>61</v>
       </c>
       <c r="C61" s="19"/>
-      <c r="D61" s="0" t="e">
+      <c r="D61" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C61,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38546,9 +39096,11 @@
         <v>62</v>
       </c>
       <c r="C62" s="13"/>
-      <c r="D62" s="0" t="e">
+      <c r="D62" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C62,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38559,9 +39111,11 @@
         <v>63</v>
       </c>
       <c r="C63" s="19"/>
-      <c r="D63" s="0" t="e">
+      <c r="D63" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C63,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38572,9 +39126,11 @@
         <v>64</v>
       </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="0" t="e">
+      <c r="D64" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C64,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="65" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38600,9 +39156,11 @@
         <v>66</v>
       </c>
       <c r="C66" s="7"/>
-      <c r="D66" s="0" t="e">
+      <c r="D66" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C66,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38613,9 +39171,11 @@
         <v>67</v>
       </c>
       <c r="C67" s="25"/>
-      <c r="D67" s="0" t="e">
+      <c r="D67" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C67,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38626,9 +39186,11 @@
         <v>68</v>
       </c>
       <c r="C68" s="25"/>
-      <c r="D68" s="0" t="e">
+      <c r="D68" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C68,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38639,9 +39201,11 @@
         <v>69</v>
       </c>
       <c r="C69" s="25"/>
-      <c r="D69" s="0" t="e">
+      <c r="D69" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C69,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38652,9 +39216,11 @@
         <v>70</v>
       </c>
       <c r="C70" s="25"/>
-      <c r="D70" s="0" t="e">
+      <c r="D70" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C70,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38665,9 +39231,11 @@
         <v>71</v>
       </c>
       <c r="C71" s="25"/>
-      <c r="D71" s="0" t="e">
+      <c r="D71" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C71,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38678,9 +39246,11 @@
         <v>72</v>
       </c>
       <c r="C72" s="25"/>
-      <c r="D72" s="0" t="e">
+      <c r="D72" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C72,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38691,9 +39261,11 @@
         <v>73</v>
       </c>
       <c r="C73" s="25"/>
-      <c r="D73" s="0" t="e">
+      <c r="D73" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C73,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38704,9 +39276,11 @@
         <v>74</v>
       </c>
       <c r="C74" s="25"/>
-      <c r="D74" s="0" t="e">
+      <c r="D74" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C74,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38717,9 +39291,11 @@
         <v>75</v>
       </c>
       <c r="C75" s="25"/>
-      <c r="D75" s="0" t="e">
+      <c r="D75" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C75,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38730,9 +39306,11 @@
         <v>76</v>
       </c>
       <c r="C76" s="25"/>
-      <c r="D76" s="0" t="e">
+      <c r="D76" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C76,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38743,9 +39321,11 @@
         <v>77</v>
       </c>
       <c r="C77" s="25"/>
-      <c r="D77" s="0" t="e">
+      <c r="D77" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C77,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38756,9 +39336,11 @@
         <v>78</v>
       </c>
       <c r="C78" s="25"/>
-      <c r="D78" s="0" t="e">
+      <c r="D78" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C78,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38769,9 +39351,11 @@
         <v>79</v>
       </c>
       <c r="C79" s="25"/>
-      <c r="D79" s="0" t="e">
+      <c r="D79" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C79,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38782,9 +39366,11 @@
         <v>80</v>
       </c>
       <c r="C80" s="25"/>
-      <c r="D80" s="0" t="e">
+      <c r="D80" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C80,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38795,9 +39381,11 @@
         <v>81</v>
       </c>
       <c r="C81" s="25"/>
-      <c r="D81" s="0" t="e">
+      <c r="D81" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C81,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38808,9 +39396,11 @@
         <v>82</v>
       </c>
       <c r="C82" s="25"/>
-      <c r="D82" s="0" t="e">
+      <c r="D82" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C82,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38821,9 +39411,11 @@
         <v>83</v>
       </c>
       <c r="C83" s="25"/>
-      <c r="D83" s="0" t="e">
+      <c r="D83" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C83,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38834,9 +39426,11 @@
         <v>84</v>
       </c>
       <c r="C84" s="25"/>
-      <c r="D84" s="0" t="e">
+      <c r="D84" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C84,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38847,9 +39441,11 @@
         <v>85</v>
       </c>
       <c r="C85" s="25"/>
-      <c r="D85" s="0" t="e">
+      <c r="D85" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C85,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38860,9 +39456,11 @@
         <v>86</v>
       </c>
       <c r="C86" s="25"/>
-      <c r="D86" s="0" t="e">
+      <c r="D86" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C86,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38873,9 +39471,11 @@
         <v>87</v>
       </c>
       <c r="C87" s="25"/>
-      <c r="D87" s="0" t="e">
+      <c r="D87" s="0" t="inlineStr">
         <f aca="false">VLOOKUP(C87,A:B,2,0)</f>
-        <v>#N/A</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>